<commit_message>
Write script for use excel Data.
</commit_message>
<xml_diff>
--- a/seleniumPractice/ExcelData/MyData.xlsx
+++ b/seleniumPractice/ExcelData/MyData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2520" windowWidth="23265" windowHeight="11160"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="16695" windowHeight="6480"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -12,6 +12,7 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725"/>
+  <oleSize ref="A1"/>
 </workbook>
 </file>
 
@@ -33,12 +34,6 @@
     <t>B</t>
   </si>
   <si>
-    <t>C</t>
-  </si>
-  <si>
-    <t>D</t>
-  </si>
-  <si>
     <t>E</t>
   </si>
   <si>
@@ -61,6 +56,12 @@
   </si>
   <si>
     <t>FF</t>
+  </si>
+  <si>
+    <t>Auntor</t>
+  </si>
+  <si>
+    <t>Acharja</t>
   </si>
 </sst>
 </file>
@@ -412,7 +413,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -441,7 +442,7 @@
         <v>3</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -452,7 +453,7 @@
         <v>4</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -460,10 +461,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -471,10 +472,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -482,10 +483,10 @@
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -493,10 +494,10 @@
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>